<commit_message>
Salesforce Bulk Api with Example
</commit_message>
<xml_diff>
--- a/me/5.Salesforce-BULK-API.xlsx
+++ b/me/5.Salesforce-BULK-API.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce-integration-with-external-systems\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58CCC10-5610-4E7F-B439-1D79DCFC2448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16770BA2-D08C-42D5-A832-9334BD6F0D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a bulk API in Salesforce" sheetId="1" r:id="rId1"/>
+    <sheet name="SalesforceBulkApiWithExample" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="119">
   <si>
     <t>構成</t>
   </si>
@@ -280,6 +281,189 @@
   </si>
   <si>
     <t>new</t>
+  </si>
+  <si>
+    <t>Insert the student records</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt; </t>
+  </si>
+  <si>
+    <t>&lt;jobInfo xmlns="http://www.force.com/2009/06/asyncapi/dataload"&gt; </t>
+  </si>
+  <si>
+    <t>    &lt;operation&gt;insert&lt;/operation&gt; </t>
+  </si>
+  <si>
+    <t>    &lt;contentType&gt;XML&lt;/contentType&gt; </t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;object&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Student__c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/object&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>Now we have 9 students</t>
+  </si>
+  <si>
+    <t>&lt;sObjects xmlns="http://www.force.com/2009/06/asyncapi/dataload"&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;sObject&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Student_Name__c&gt; Lovish Bajaj &lt;/Student_Name__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Phone_Number__c&gt;7890987777&lt;/Phone_Number__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Email__c&gt;lovish@yahoo.com&lt;/Email__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Address__c&gt;India&lt;/Address__c&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/sObject&gt;</t>
+  </si>
+  <si>
+    <t>     &lt;sObject&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Student_Name__c&gt; Sahil Khan &lt;/Student_Name__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Phone_Number__c&gt;3130987777&lt;/Phone_Number__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Email__c&gt;sahil_khan@yahoo.com&lt;/Email__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Address__c&gt;Pakistan&lt;/Address__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Student_Name__c&gt; Neha Sidana &lt;/Student_Name__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Phone_Number__c&gt;7678987777&lt;/Phone_Number__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Email__c&gt;nehasidana@gmail.com&lt;/Email__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Address__c&gt;Canada&lt;/Address__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Student_Name__c&gt; Prerna Sharma&lt;/Student_Name__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Phone_Number__c&gt;7760987777&lt;/Phone_Number__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Email__c&gt;prernasharma112@yahoo.com&lt;/Email__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Address__c&gt;Austin,Texas&lt;/Address__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Student_Name__c&gt; Ishita Saxena &lt;/Student_Name__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Phone_Number__c&gt;7865432222&lt;/Phone_Number__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Email__c&gt;ishita56@yahoo.com&lt;/Email__c&gt;</t>
+  </si>
+  <si>
+    <t>       &lt;Address__c&gt;Dallas,Texas&lt;/Address__c&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Queued</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> means it has still not process, but it will take its time because it is an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>asynchronous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> process. It is not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>synchronous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. It will take the time</t>
+    </r>
+  </si>
+  <si>
+    <t>records have been inserted</t>
+  </si>
+  <si>
+    <t>We do not have any more records to insert so we can close this job</t>
   </si>
 </sst>
 </file>
@@ -408,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -421,6 +605,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2447,6 +2643,645 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295594</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA9D4227-9C02-A239-5B2B-3269AEAD67AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695324" y="4276725"/>
+          <a:ext cx="9353870" cy="4914900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>8309</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>56850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C269B5-782A-EB19-3994-79E96E138EE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="647700" y="10991850"/>
+          <a:ext cx="9723809" cy="2400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>68096</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1113795D-401F-F8D6-4089-2EF70AB69411}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="13630275"/>
+          <a:ext cx="9915525" cy="4725821"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>353786</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>40291</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9887ED-FCD2-BE7D-BD2F-5469AD60243A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="717096" y="18573751"/>
+          <a:ext cx="11270797" cy="5660040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>118880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{332E210F-2897-D94A-E7D1-995D8D360DAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="24660225"/>
+          <a:ext cx="10963275" cy="5176655"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>65457</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>18340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73CDAD80-4F19-8898-AE0C-7753B55C7F95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="36633150"/>
+          <a:ext cx="9742857" cy="5676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>224</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>427446</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>47257</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92C853A8-71D1-B002-E69F-9EC758E78A3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="42824400"/>
+          <a:ext cx="9428571" cy="2942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>272</xdr:row>
+      <xdr:rowOff>31691</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FE0A947-84A4-7EF3-DF7B-A862452550D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="46377225"/>
+          <a:ext cx="10467975" cy="5279966"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>273</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>86235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B18CB16-BA7C-8458-2BB5-37235DAE2367}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="52044601"/>
+          <a:ext cx="11210925" cy="5572634"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>41781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28BB0174-7135-1D60-DAD4-F77EE7B5F132}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="58407300"/>
+          <a:ext cx="11334750" cy="5642481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>41823</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D9DB8F-8C7D-C1E3-7850-9F467BC8F52B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="64322325"/>
+          <a:ext cx="11315700" cy="5632998"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>368</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>398</xdr:row>
+      <xdr:rowOff>39076</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{241BDEF8-8B63-92A0-A989-CC8CD3A324E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="70189725"/>
+          <a:ext cx="11287125" cy="5668351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>399</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>429</xdr:row>
+      <xdr:rowOff>39119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07F7661E-1247-BFC3-BC90-9468D0DFE88A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="76085701"/>
+          <a:ext cx="11306175" cy="5677918"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>430</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>460</xdr:row>
+      <xdr:rowOff>64058</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5411E87-C0F0-5B2D-24D8-72718DDBB50E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="709893" y="82019775"/>
+          <a:ext cx="11168342" cy="5674283"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2717,8 +3552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R687"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A427" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A437" sqref="A437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,4 +4210,711 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A74976-4CE2-4DCE-A370-55CD7B286193}">
+  <dimension ref="A2:I306"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I463" sqref="I463"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="9"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B160" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C160" s="3"/>
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
+      <c r="H160" s="3"/>
+      <c r="I160" s="4"/>
+    </row>
+    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B161" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C161" s="22"/>
+      <c r="D161" s="22"/>
+      <c r="E161" s="22"/>
+      <c r="F161" s="22"/>
+      <c r="G161" s="22"/>
+      <c r="H161" s="22"/>
+      <c r="I161" s="6"/>
+    </row>
+    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B162" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C162" s="22"/>
+      <c r="D162" s="22"/>
+      <c r="E162" s="22"/>
+      <c r="F162" s="22"/>
+      <c r="G162" s="22"/>
+      <c r="H162" s="22"/>
+      <c r="I162" s="6"/>
+    </row>
+    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B163" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C163" s="22"/>
+      <c r="D163" s="22"/>
+      <c r="E163" s="22"/>
+      <c r="F163" s="22"/>
+      <c r="G163" s="22"/>
+      <c r="H163" s="22"/>
+      <c r="I163" s="6"/>
+    </row>
+    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B164" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C164" s="22"/>
+      <c r="D164" s="22"/>
+      <c r="E164" s="22"/>
+      <c r="F164" s="22"/>
+      <c r="G164" s="22"/>
+      <c r="H164" s="22"/>
+      <c r="I164" s="6"/>
+    </row>
+    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B165" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C165" s="22"/>
+      <c r="D165" s="22"/>
+      <c r="E165" s="22"/>
+      <c r="F165" s="22"/>
+      <c r="G165" s="22"/>
+      <c r="H165" s="22"/>
+      <c r="I165" s="6"/>
+    </row>
+    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B166" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C166" s="22"/>
+      <c r="D166" s="22"/>
+      <c r="E166" s="22"/>
+      <c r="F166" s="22"/>
+      <c r="G166" s="22"/>
+      <c r="H166" s="22"/>
+      <c r="I166" s="6"/>
+    </row>
+    <row r="167" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B167" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C167" s="22"/>
+      <c r="D167" s="22"/>
+      <c r="E167" s="22"/>
+      <c r="F167" s="22"/>
+      <c r="G167" s="22"/>
+      <c r="H167" s="22"/>
+      <c r="I167" s="6"/>
+    </row>
+    <row r="168" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B168" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C168" s="22"/>
+      <c r="D168" s="22"/>
+      <c r="E168" s="22"/>
+      <c r="F168" s="22"/>
+      <c r="G168" s="22"/>
+      <c r="H168" s="22"/>
+      <c r="I168" s="6"/>
+    </row>
+    <row r="169" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B169" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C169" s="22"/>
+      <c r="D169" s="22"/>
+      <c r="E169" s="22"/>
+      <c r="F169" s="22"/>
+      <c r="G169" s="22"/>
+      <c r="H169" s="22"/>
+      <c r="I169" s="6"/>
+    </row>
+    <row r="170" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B170" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C170" s="22"/>
+      <c r="D170" s="22"/>
+      <c r="E170" s="22"/>
+      <c r="F170" s="22"/>
+      <c r="G170" s="22"/>
+      <c r="H170" s="22"/>
+      <c r="I170" s="6"/>
+    </row>
+    <row r="171" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B171" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C171" s="22"/>
+      <c r="D171" s="22"/>
+      <c r="E171" s="22"/>
+      <c r="F171" s="22"/>
+      <c r="G171" s="22"/>
+      <c r="H171" s="22"/>
+      <c r="I171" s="6"/>
+    </row>
+    <row r="172" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B172" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C172" s="22"/>
+      <c r="D172" s="22"/>
+      <c r="E172" s="22"/>
+      <c r="F172" s="22"/>
+      <c r="G172" s="22"/>
+      <c r="H172" s="22"/>
+      <c r="I172" s="6"/>
+    </row>
+    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B173" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C173" s="22"/>
+      <c r="D173" s="22"/>
+      <c r="E173" s="22"/>
+      <c r="F173" s="22"/>
+      <c r="G173" s="22"/>
+      <c r="H173" s="22"/>
+      <c r="I173" s="6"/>
+    </row>
+    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B174" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C174" s="22"/>
+      <c r="D174" s="22"/>
+      <c r="E174" s="22"/>
+      <c r="F174" s="22"/>
+      <c r="G174" s="22"/>
+      <c r="H174" s="22"/>
+      <c r="I174" s="6"/>
+    </row>
+    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B175" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C175" s="22"/>
+      <c r="D175" s="22"/>
+      <c r="E175" s="22"/>
+      <c r="F175" s="22"/>
+      <c r="G175" s="22"/>
+      <c r="H175" s="22"/>
+      <c r="I175" s="6"/>
+    </row>
+    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B176" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C176" s="22"/>
+      <c r="D176" s="22"/>
+      <c r="E176" s="22"/>
+      <c r="F176" s="22"/>
+      <c r="G176" s="22"/>
+      <c r="H176" s="22"/>
+      <c r="I176" s="6"/>
+    </row>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B177" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C177" s="22"/>
+      <c r="D177" s="22"/>
+      <c r="E177" s="22"/>
+      <c r="F177" s="22"/>
+      <c r="G177" s="22"/>
+      <c r="H177" s="22"/>
+      <c r="I177" s="6"/>
+    </row>
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B178" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C178" s="22"/>
+      <c r="D178" s="22"/>
+      <c r="E178" s="22"/>
+      <c r="F178" s="22"/>
+      <c r="G178" s="22"/>
+      <c r="H178" s="22"/>
+      <c r="I178" s="6"/>
+    </row>
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B179" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C179" s="22"/>
+      <c r="D179" s="22"/>
+      <c r="E179" s="22"/>
+      <c r="F179" s="22"/>
+      <c r="G179" s="22"/>
+      <c r="H179" s="22"/>
+      <c r="I179" s="6"/>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B180" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C180" s="22"/>
+      <c r="D180" s="22"/>
+      <c r="E180" s="22"/>
+      <c r="F180" s="22"/>
+      <c r="G180" s="22"/>
+      <c r="H180" s="22"/>
+      <c r="I180" s="6"/>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B181" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C181" s="22"/>
+      <c r="D181" s="22"/>
+      <c r="E181" s="22"/>
+      <c r="F181" s="22"/>
+      <c r="G181" s="22"/>
+      <c r="H181" s="22"/>
+      <c r="I181" s="6"/>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B182" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C182" s="22"/>
+      <c r="D182" s="22"/>
+      <c r="E182" s="22"/>
+      <c r="F182" s="22"/>
+      <c r="G182" s="22"/>
+      <c r="H182" s="22"/>
+      <c r="I182" s="6"/>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B183" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C183" s="22"/>
+      <c r="D183" s="22"/>
+      <c r="E183" s="22"/>
+      <c r="F183" s="22"/>
+      <c r="G183" s="22"/>
+      <c r="H183" s="22"/>
+      <c r="I183" s="6"/>
+    </row>
+    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B184" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C184" s="22"/>
+      <c r="D184" s="22"/>
+      <c r="E184" s="22"/>
+      <c r="F184" s="22"/>
+      <c r="G184" s="22"/>
+      <c r="H184" s="22"/>
+      <c r="I184" s="6"/>
+    </row>
+    <row r="185" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B185" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C185" s="22"/>
+      <c r="D185" s="22"/>
+      <c r="E185" s="22"/>
+      <c r="F185" s="22"/>
+      <c r="G185" s="22"/>
+      <c r="H185" s="22"/>
+      <c r="I185" s="6"/>
+    </row>
+    <row r="186" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B186" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C186" s="22"/>
+      <c r="D186" s="22"/>
+      <c r="E186" s="22"/>
+      <c r="F186" s="22"/>
+      <c r="G186" s="22"/>
+      <c r="H186" s="22"/>
+      <c r="I186" s="6"/>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B187" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C187" s="22"/>
+      <c r="D187" s="22"/>
+      <c r="E187" s="22"/>
+      <c r="F187" s="22"/>
+      <c r="G187" s="22"/>
+      <c r="H187" s="22"/>
+      <c r="I187" s="6"/>
+    </row>
+    <row r="188" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B188" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C188" s="22"/>
+      <c r="D188" s="22"/>
+      <c r="E188" s="22"/>
+      <c r="F188" s="22"/>
+      <c r="G188" s="22"/>
+      <c r="H188" s="22"/>
+      <c r="I188" s="6"/>
+    </row>
+    <row r="189" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B189" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C189" s="22"/>
+      <c r="D189" s="22"/>
+      <c r="E189" s="22"/>
+      <c r="F189" s="22"/>
+      <c r="G189" s="22"/>
+      <c r="H189" s="22"/>
+      <c r="I189" s="6"/>
+    </row>
+    <row r="190" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B190" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C190" s="22"/>
+      <c r="D190" s="22"/>
+      <c r="E190" s="22"/>
+      <c r="F190" s="22"/>
+      <c r="G190" s="22"/>
+      <c r="H190" s="22"/>
+      <c r="I190" s="6"/>
+    </row>
+    <row r="191" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B191" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C191" s="8"/>
+      <c r="D191" s="8"/>
+      <c r="E191" s="8"/>
+      <c r="F191" s="8"/>
+      <c r="G191" s="8"/>
+      <c r="H191" s="8"/>
+      <c r="I191" s="9"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="23"/>
+      <c r="B244" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B306" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Salesforce Bulk API: Upload records using a CSV file in salesforce
</commit_message>
<xml_diff>
--- a/me/5.Salesforce-BULK-API.xlsx
+++ b/me/5.Salesforce-BULK-API.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce-integration-with-external-systems\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16770BA2-D08C-42D5-A832-9334BD6F0D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661F3359-6933-45C7-A464-6E05C9F7E969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a bulk API in Salesforce" sheetId="1" r:id="rId1"/>
     <sheet name="SalesforceBulkApiWithExample" sheetId="2" r:id="rId2"/>
+    <sheet name="Upload records using a CSV file" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="161">
   <si>
     <t>構成</t>
   </si>
@@ -321,9 +322,6 @@
       </rPr>
       <t>&lt;/object&gt; </t>
     </r>
-  </si>
-  <si>
-    <t>Now we have 9 students</t>
   </si>
   <si>
     <t>&lt;sObjects xmlns="http://www.force.com/2009/06/asyncapi/dataload"&gt;</t>
@@ -464,6 +462,157 @@
   </si>
   <si>
     <t>We do not have any more records to insert so we can close this job</t>
+  </si>
+  <si>
+    <t>1.Create-a-bulk-API-in-Salesforce</t>
+  </si>
+  <si>
+    <t>2.Salesforce-Bulk-Api-with-Example</t>
+  </si>
+  <si>
+    <t>3.Upload-records-using-a-CSV-file</t>
+  </si>
+  <si>
+    <t>StudentFile.xlsx</t>
+  </si>
+  <si>
+    <t>StudentFile.csv</t>
+  </si>
+  <si>
+    <t>salesforce-integration-with-external-systems\5.Salesforce-BULK-API\3.Upload-records-using-a-CSV-file\CreateJobInsertStudentRecordsViaCSV.txt</t>
+  </si>
+  <si>
+    <t>    &lt;object&gt;Student__c&lt;/object&gt; </t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;contentType&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CSV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/contentType&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;jobInfo</t>
+  </si>
+  <si>
+    <t>    &lt;id&gt;7505g00000IHNamAAH&lt;/id&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;operation&gt;insert&lt;/operation&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;object&gt;Student__c&lt;/object&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;createdById&gt;0055g00000EjhCCAAZ&lt;/createdById&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;createdDate&gt;2023-02-14T15:38:04.000Z&lt;/createdDate&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;systemModstamp&gt;2023-02-14T15:38:04.000Z&lt;/systemModstamp&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;state&gt;Open&lt;/state&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;concurrencyMode&gt;Parallel&lt;/concurrencyMode&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;contentType&gt;CSV&lt;/contentType&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;numberBatchesQueued&gt;0&lt;/numberBatchesQueued&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;numberBatchesInProgress&gt;0&lt;/numberBatchesInProgress&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;numberBatchesCompleted&gt;0&lt;/numberBatchesCompleted&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;numberBatchesFailed&gt;0&lt;/numberBatchesFailed&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;numberBatchesTotal&gt;0&lt;/numberBatchesTotal&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;numberRetries&gt;0&lt;/numberRetries&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;apiVersion&gt;57.0&lt;/apiVersion&gt;</t>
+  </si>
+  <si>
+    <t>This part we will upload csv file has the same exact field names that we have in Salesforce</t>
+  </si>
+  <si>
+    <t>We will upload csv file has the same exact field names that we have in Salesforce</t>
+  </si>
+  <si>
+    <t>salesforce-integration-with-external-systems\5.Salesforce-BULK-API\3.Upload-records-using-a-CSV-file\StudentFile.csv</t>
+  </si>
+  <si>
+    <t>Student_Name__c</t>
+  </si>
+  <si>
+    <t>Phone_Number__c</t>
+  </si>
+  <si>
+    <t>Address__c</t>
+  </si>
+  <si>
+    <t>Email__c</t>
+  </si>
+  <si>
+    <t>Rakshita Bhojwani</t>
+  </si>
+  <si>
+    <t>Toronto, Canada</t>
+  </si>
+  <si>
+    <t>bhojwani@gmail.com</t>
+  </si>
+  <si>
+    <t>Vinay Sandhu</t>
+  </si>
+  <si>
+    <t>Newzealand</t>
+  </si>
+  <si>
+    <t>viany@yahoo.com</t>
+  </si>
+  <si>
+    <t>Daman Preeet</t>
+  </si>
+  <si>
+    <t>Vancouver, Canada</t>
+  </si>
+  <si>
+    <t>preet_daman@hotmail.com</t>
+  </si>
+  <si>
+    <t>Now we have 9 students(before insert)</t>
+  </si>
+  <si>
+    <t>Now we have 14 students(before insert)</t>
   </si>
 </sst>
 </file>
@@ -592,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -605,18 +754,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3282,6 +3420,786 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>10697</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A29CFDC-4687-615B-3F6E-467DD41AE8B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="5248274"/>
+          <a:ext cx="9982200" cy="5239923"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>294107</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>9211</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09A1D3CB-DA3E-782B-5DAF-5328549BD6E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="12544425"/>
+          <a:ext cx="9342857" cy="2514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>303628</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>37773</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C624E140-A4EC-6E5D-343A-DA0007E2E6CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="15325725"/>
+          <a:ext cx="9371428" cy="2619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>103557</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>189889</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{847E0275-D899-9700-EBE5-4437AFF79CC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="18164175"/>
+          <a:ext cx="9742857" cy="4885714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>58560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00A3A160-B0F9-C52D-197D-71B0E2BC2BF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="28146376"/>
+          <a:ext cx="11163300" cy="5630684"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>187457</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4ACD6A3-6E12-2DD3-728A-8AC4C9BCA5FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="35775900"/>
+          <a:ext cx="9864857" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>68849</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEF438BB-0D15-C04B-1C71-F08CFB140036}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="34394775"/>
+          <a:ext cx="9753600" cy="5298074"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>122605</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>18844</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B612EC4E-57F6-00F4-9D1E-E935228275F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="44281725"/>
+          <a:ext cx="9761905" cy="1647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>160705</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>114075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F83D08A-1B52-DB57-069C-EFD921902D8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="46129575"/>
+          <a:ext cx="9761905" cy="1800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>113084</xdr:colOff>
+      <xdr:row>301</xdr:row>
+      <xdr:rowOff>47252</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4F4BBF9-C4BC-4C0E-4584-1309D320F4A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="48120300"/>
+          <a:ext cx="9723809" cy="2980952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>194022</xdr:colOff>
+      <xdr:row>249</xdr:row>
+      <xdr:rowOff>98549</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0156A6DB-9B1D-4C62-A4A3-6A3BCEC87AB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="728383" y="41618647"/>
+          <a:ext cx="10962874" cy="5914402"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>259317</xdr:colOff>
+      <xdr:row>318</xdr:row>
+      <xdr:rowOff>19235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AB41774-4009-027D-2591-A385EEFEA4F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="784412" y="57598235"/>
+          <a:ext cx="9761905" cy="3000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>322</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>357</xdr:row>
+      <xdr:rowOff>72238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{486B0C78-F88C-545F-1E18-CF526F695D2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="728383" y="61430647"/>
+          <a:ext cx="10892117" cy="6650091"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>112058</xdr:colOff>
+      <xdr:row>360</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>347383</xdr:colOff>
+      <xdr:row>390</xdr:row>
+      <xdr:rowOff>6596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{961D4BA1-BAC8-B6CD-F799-ACAB33EE0908}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="717176" y="68680853"/>
+          <a:ext cx="11127442" cy="5620743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>391</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>4766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7674994E-B32F-9E43-A3D5-329DA98F562F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="683559" y="74575147"/>
+          <a:ext cx="11194676" cy="5630119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>89648</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>451</xdr:row>
+      <xdr:rowOff>38121</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1D75703-0C36-F7E2-BD6D-00957513D14C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="694766" y="80368589"/>
+          <a:ext cx="11105028" cy="5585032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>504264</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>112058</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{194DF50B-86C4-29BB-91FE-1B43E0E169EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1109382" y="4347882"/>
+          <a:ext cx="1423147" cy="47389677"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4216,8 +5134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A74976-4CE2-4DCE-A370-55CD7B286193}">
   <dimension ref="A2:I306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I463" sqref="I463"/>
+    <sheetView topLeftCell="A343" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A305" sqref="A305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4228,194 +5146,120 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="18"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="18"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="18"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="5"/>
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="18"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
+      <c r="B10" s="5"/>
+      <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="18"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
+      <c r="B11" s="5"/>
+      <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="18"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
+      <c r="B12" s="5"/>
+      <c r="E12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="18"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
+      <c r="B13" s="5"/>
+      <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="18"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13" t="s">
+      <c r="B14" s="5"/>
+      <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="18"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13" t="s">
+      <c r="B15" s="5"/>
+      <c r="F15" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="18"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13" t="s">
+      <c r="B16" s="5"/>
+      <c r="F16" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="18"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13" t="s">
+      <c r="B17" s="5"/>
+      <c r="F17" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="18"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="18"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -4442,44 +5286,24 @@
       <c r="B53" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
       <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
       <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
       <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
       <c r="H56" s="6"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -4495,7 +5319,7 @@
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -4505,7 +5329,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B160" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
@@ -4517,362 +5341,182 @@
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B161" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C161" s="22"/>
-      <c r="D161" s="22"/>
-      <c r="E161" s="22"/>
-      <c r="F161" s="22"/>
-      <c r="G161" s="22"/>
-      <c r="H161" s="22"/>
+        <v>92</v>
+      </c>
       <c r="I161" s="6"/>
     </row>
     <row r="162" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B162" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C162" s="22"/>
-      <c r="D162" s="22"/>
-      <c r="E162" s="22"/>
-      <c r="F162" s="22"/>
-      <c r="G162" s="22"/>
-      <c r="H162" s="22"/>
+        <v>93</v>
+      </c>
       <c r="I162" s="6"/>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B163" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C163" s="22"/>
-      <c r="D163" s="22"/>
-      <c r="E163" s="22"/>
-      <c r="F163" s="22"/>
-      <c r="G163" s="22"/>
-      <c r="H163" s="22"/>
+        <v>94</v>
+      </c>
       <c r="I163" s="6"/>
     </row>
     <row r="164" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B164" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C164" s="22"/>
-      <c r="D164" s="22"/>
-      <c r="E164" s="22"/>
-      <c r="F164" s="22"/>
-      <c r="G164" s="22"/>
-      <c r="H164" s="22"/>
+        <v>95</v>
+      </c>
       <c r="I164" s="6"/>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B165" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C165" s="22"/>
-      <c r="D165" s="22"/>
-      <c r="E165" s="22"/>
-      <c r="F165" s="22"/>
-      <c r="G165" s="22"/>
-      <c r="H165" s="22"/>
+        <v>96</v>
+      </c>
       <c r="I165" s="6"/>
     </row>
     <row r="166" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B166" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C166" s="22"/>
-      <c r="D166" s="22"/>
-      <c r="E166" s="22"/>
-      <c r="F166" s="22"/>
-      <c r="G166" s="22"/>
-      <c r="H166" s="22"/>
+        <v>97</v>
+      </c>
       <c r="I166" s="6"/>
     </row>
     <row r="167" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B167" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C167" s="22"/>
-      <c r="D167" s="22"/>
-      <c r="E167" s="22"/>
-      <c r="F167" s="22"/>
-      <c r="G167" s="22"/>
-      <c r="H167" s="22"/>
+        <v>98</v>
+      </c>
       <c r="I167" s="6"/>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B168" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C168" s="22"/>
-      <c r="D168" s="22"/>
-      <c r="E168" s="22"/>
-      <c r="F168" s="22"/>
-      <c r="G168" s="22"/>
-      <c r="H168" s="22"/>
+        <v>99</v>
+      </c>
       <c r="I168" s="6"/>
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B169" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C169" s="22"/>
-      <c r="D169" s="22"/>
-      <c r="E169" s="22"/>
-      <c r="F169" s="22"/>
-      <c r="G169" s="22"/>
-      <c r="H169" s="22"/>
+        <v>100</v>
+      </c>
       <c r="I169" s="6"/>
     </row>
     <row r="170" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B170" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C170" s="22"/>
-      <c r="D170" s="22"/>
-      <c r="E170" s="22"/>
-      <c r="F170" s="22"/>
-      <c r="G170" s="22"/>
-      <c r="H170" s="22"/>
+        <v>101</v>
+      </c>
       <c r="I170" s="6"/>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B171" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C171" s="22"/>
-      <c r="D171" s="22"/>
-      <c r="E171" s="22"/>
-      <c r="F171" s="22"/>
-      <c r="G171" s="22"/>
-      <c r="H171" s="22"/>
+        <v>102</v>
+      </c>
       <c r="I171" s="6"/>
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B172" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C172" s="22"/>
-      <c r="D172" s="22"/>
-      <c r="E172" s="22"/>
-      <c r="F172" s="22"/>
-      <c r="G172" s="22"/>
-      <c r="H172" s="22"/>
+        <v>97</v>
+      </c>
       <c r="I172" s="6"/>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B173" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C173" s="22"/>
-      <c r="D173" s="22"/>
-      <c r="E173" s="22"/>
-      <c r="F173" s="22"/>
-      <c r="G173" s="22"/>
-      <c r="H173" s="22"/>
+        <v>98</v>
+      </c>
       <c r="I173" s="6"/>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B174" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C174" s="22"/>
-      <c r="D174" s="22"/>
-      <c r="E174" s="22"/>
-      <c r="F174" s="22"/>
-      <c r="G174" s="22"/>
-      <c r="H174" s="22"/>
+        <v>103</v>
+      </c>
       <c r="I174" s="6"/>
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B175" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C175" s="22"/>
-      <c r="D175" s="22"/>
-      <c r="E175" s="22"/>
-      <c r="F175" s="22"/>
-      <c r="G175" s="22"/>
-      <c r="H175" s="22"/>
+        <v>104</v>
+      </c>
       <c r="I175" s="6"/>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B176" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C176" s="22"/>
-      <c r="D176" s="22"/>
-      <c r="E176" s="22"/>
-      <c r="F176" s="22"/>
-      <c r="G176" s="22"/>
-      <c r="H176" s="22"/>
+        <v>105</v>
+      </c>
       <c r="I176" s="6"/>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B177" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C177" s="22"/>
-      <c r="D177" s="22"/>
-      <c r="E177" s="22"/>
-      <c r="F177" s="22"/>
-      <c r="G177" s="22"/>
-      <c r="H177" s="22"/>
+        <v>106</v>
+      </c>
       <c r="I177" s="6"/>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B178" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C178" s="22"/>
-      <c r="D178" s="22"/>
-      <c r="E178" s="22"/>
-      <c r="F178" s="22"/>
-      <c r="G178" s="22"/>
-      <c r="H178" s="22"/>
+        <v>97</v>
+      </c>
       <c r="I178" s="6"/>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B179" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C179" s="22"/>
-      <c r="D179" s="22"/>
-      <c r="E179" s="22"/>
-      <c r="F179" s="22"/>
-      <c r="G179" s="22"/>
-      <c r="H179" s="22"/>
+        <v>98</v>
+      </c>
       <c r="I179" s="6"/>
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B180" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C180" s="22"/>
-      <c r="D180" s="22"/>
-      <c r="E180" s="22"/>
-      <c r="F180" s="22"/>
-      <c r="G180" s="22"/>
-      <c r="H180" s="22"/>
+        <v>107</v>
+      </c>
       <c r="I180" s="6"/>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B181" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C181" s="22"/>
-      <c r="D181" s="22"/>
-      <c r="E181" s="22"/>
-      <c r="F181" s="22"/>
-      <c r="G181" s="22"/>
-      <c r="H181" s="22"/>
+        <v>108</v>
+      </c>
       <c r="I181" s="6"/>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B182" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C182" s="22"/>
-      <c r="D182" s="22"/>
-      <c r="E182" s="22"/>
-      <c r="F182" s="22"/>
-      <c r="G182" s="22"/>
-      <c r="H182" s="22"/>
+        <v>109</v>
+      </c>
       <c r="I182" s="6"/>
     </row>
     <row r="183" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B183" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C183" s="22"/>
-      <c r="D183" s="22"/>
-      <c r="E183" s="22"/>
-      <c r="F183" s="22"/>
-      <c r="G183" s="22"/>
-      <c r="H183" s="22"/>
+        <v>110</v>
+      </c>
       <c r="I183" s="6"/>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B184" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C184" s="22"/>
-      <c r="D184" s="22"/>
-      <c r="E184" s="22"/>
-      <c r="F184" s="22"/>
-      <c r="G184" s="22"/>
-      <c r="H184" s="22"/>
+        <v>97</v>
+      </c>
       <c r="I184" s="6"/>
     </row>
     <row r="185" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B185" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C185" s="22"/>
-      <c r="D185" s="22"/>
-      <c r="E185" s="22"/>
-      <c r="F185" s="22"/>
-      <c r="G185" s="22"/>
-      <c r="H185" s="22"/>
+        <v>98</v>
+      </c>
       <c r="I185" s="6"/>
     </row>
     <row r="186" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B186" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C186" s="22"/>
-      <c r="D186" s="22"/>
-      <c r="E186" s="22"/>
-      <c r="F186" s="22"/>
-      <c r="G186" s="22"/>
-      <c r="H186" s="22"/>
+        <v>111</v>
+      </c>
       <c r="I186" s="6"/>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B187" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C187" s="22"/>
-      <c r="D187" s="22"/>
-      <c r="E187" s="22"/>
-      <c r="F187" s="22"/>
-      <c r="G187" s="22"/>
-      <c r="H187" s="22"/>
+        <v>112</v>
+      </c>
       <c r="I187" s="6"/>
     </row>
     <row r="188" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B188" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C188" s="22"/>
-      <c r="D188" s="22"/>
-      <c r="E188" s="22"/>
-      <c r="F188" s="22"/>
-      <c r="G188" s="22"/>
-      <c r="H188" s="22"/>
+        <v>113</v>
+      </c>
       <c r="I188" s="6"/>
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B189" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C189" s="22"/>
-      <c r="D189" s="22"/>
-      <c r="E189" s="22"/>
-      <c r="F189" s="22"/>
-      <c r="G189" s="22"/>
-      <c r="H189" s="22"/>
+        <v>114</v>
+      </c>
       <c r="I189" s="6"/>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B190" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C190" s="22"/>
-      <c r="D190" s="22"/>
-      <c r="E190" s="22"/>
-      <c r="F190" s="22"/>
-      <c r="G190" s="22"/>
-      <c r="H190" s="22"/>
+        <v>97</v>
+      </c>
       <c r="I190" s="6"/>
     </row>
     <row r="191" spans="2:9" x14ac:dyDescent="0.25">
@@ -4889,7 +5533,7 @@
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -4898,9 +5542,8 @@
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="23"/>
       <c r="B244" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -4910,11 +5553,903 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFA91D4-86DC-4D20-9AE8-2AE8F292D674}">
+  <dimension ref="A2:I360"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W351" sqref="W351"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="D22" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="E23" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="9"/>
+    </row>
+    <row r="124" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C124" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3"/>
+      <c r="I124" s="4"/>
+    </row>
+    <row r="125" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C125" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
+      <c r="G125" s="12"/>
+      <c r="H125" s="12"/>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C126" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
+      <c r="I126" s="6"/>
+    </row>
+    <row r="127" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C127" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
+      <c r="I127" s="6"/>
+    </row>
+    <row r="128" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C128" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
+      <c r="F128" s="12"/>
+      <c r="G128" s="12"/>
+      <c r="H128" s="12"/>
+      <c r="I128" s="6"/>
+    </row>
+    <row r="129" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C129" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
+      <c r="G129" s="12"/>
+      <c r="H129" s="12"/>
+      <c r="I129" s="6"/>
+    </row>
+    <row r="130" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C130" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
+      <c r="G130" s="12"/>
+      <c r="H130" s="12"/>
+      <c r="I130" s="6"/>
+    </row>
+    <row r="131" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C131" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12"/>
+      <c r="G131" s="12"/>
+      <c r="H131" s="12"/>
+      <c r="I131" s="6"/>
+    </row>
+    <row r="132" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C132" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
+      <c r="G132" s="12"/>
+      <c r="H132" s="12"/>
+      <c r="I132" s="6"/>
+    </row>
+    <row r="133" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C133" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
+      <c r="F133" s="12"/>
+      <c r="G133" s="12"/>
+      <c r="H133" s="12"/>
+      <c r="I133" s="6"/>
+    </row>
+    <row r="134" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C134" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
+      <c r="G134" s="12"/>
+      <c r="H134" s="12"/>
+      <c r="I134" s="6"/>
+    </row>
+    <row r="135" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C135" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
+      <c r="G135" s="12"/>
+      <c r="H135" s="12"/>
+      <c r="I135" s="6"/>
+    </row>
+    <row r="136" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C136" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
+      <c r="F136" s="12"/>
+      <c r="G136" s="12"/>
+      <c r="H136" s="12"/>
+      <c r="I136" s="6"/>
+    </row>
+    <row r="137" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C137" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
+      <c r="G137" s="12"/>
+      <c r="H137" s="12"/>
+      <c r="I137" s="6"/>
+    </row>
+    <row r="138" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C138" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="6"/>
+    </row>
+    <row r="139" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C139" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="12"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="6"/>
+    </row>
+    <row r="140" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C140" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="12"/>
+      <c r="H140" s="12"/>
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C141" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D141" s="12"/>
+      <c r="E141" s="12"/>
+      <c r="F141" s="12"/>
+      <c r="G141" s="12"/>
+      <c r="H141" s="12"/>
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C142" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D142" s="12"/>
+      <c r="E142" s="12"/>
+      <c r="F142" s="12"/>
+      <c r="G142" s="12"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="6"/>
+    </row>
+    <row r="143" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C143" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
+      <c r="G143" s="12"/>
+      <c r="H143" s="12"/>
+      <c r="I143" s="6"/>
+    </row>
+    <row r="144" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C144" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D144" s="12"/>
+      <c r="E144" s="12"/>
+      <c r="F144" s="12"/>
+      <c r="G144" s="12"/>
+      <c r="H144" s="12"/>
+      <c r="I144" s="6"/>
+    </row>
+    <row r="145" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C145" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D145" s="12"/>
+      <c r="E145" s="12"/>
+      <c r="F145" s="12"/>
+      <c r="G145" s="12"/>
+      <c r="H145" s="12"/>
+      <c r="I145" s="6"/>
+    </row>
+    <row r="146" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C146" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D146" s="12"/>
+      <c r="E146" s="12"/>
+      <c r="F146" s="12"/>
+      <c r="G146" s="12"/>
+      <c r="H146" s="12"/>
+      <c r="I146" s="6"/>
+    </row>
+    <row r="147" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C147" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D147" s="12"/>
+      <c r="E147" s="12"/>
+      <c r="F147" s="12"/>
+      <c r="G147" s="12"/>
+      <c r="H147" s="12"/>
+      <c r="I147" s="6"/>
+    </row>
+    <row r="148" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C148" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D148" s="8"/>
+      <c r="E148" s="8"/>
+      <c r="F148" s="8"/>
+      <c r="G148" s="8"/>
+      <c r="H148" s="8"/>
+      <c r="I148" s="9"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B214" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F214" s="3"/>
+      <c r="G214" s="4"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B215" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C215" s="12">
+        <v>123456789</v>
+      </c>
+      <c r="D215" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E215" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F215" s="12"/>
+      <c r="G215" s="6"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B216" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C216" s="12">
+        <v>2345556767</v>
+      </c>
+      <c r="D216" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E216" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F216" s="12"/>
+      <c r="G216" s="6"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B217" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C217" s="8">
+        <v>345678901</v>
+      </c>
+      <c r="D217" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E217" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F217" s="8"/>
+      <c r="G217" s="9"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B218" s="12"/>
+      <c r="C218" s="12"/>
+      <c r="D218" s="12"/>
+      <c r="E218" s="12"/>
+      <c r="F218" s="12"/>
+      <c r="G218" s="12"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B219" s="12"/>
+      <c r="C219" s="12"/>
+      <c r="D219" s="12"/>
+      <c r="E219" s="12"/>
+      <c r="F219" s="12"/>
+      <c r="G219" s="12"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B220" s="12"/>
+      <c r="C220" s="12"/>
+      <c r="D220" s="12"/>
+      <c r="E220" s="12"/>
+      <c r="F220" s="12"/>
+      <c r="G220" s="12"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B221" s="12"/>
+      <c r="C221" s="12"/>
+      <c r="D221" s="12"/>
+      <c r="E221" s="12"/>
+      <c r="F221" s="12"/>
+      <c r="G221" s="12"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B222" s="12"/>
+      <c r="C222" s="12"/>
+      <c r="D222" s="12"/>
+      <c r="E222" s="12"/>
+      <c r="F222" s="12"/>
+      <c r="G222" s="12"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B223" s="12"/>
+      <c r="C223" s="12"/>
+      <c r="D223" s="12"/>
+      <c r="E223" s="12"/>
+      <c r="F223" s="12"/>
+      <c r="G223" s="12"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B224" s="12"/>
+      <c r="C224" s="12"/>
+      <c r="D224" s="12"/>
+      <c r="E224" s="12"/>
+      <c r="F224" s="12"/>
+      <c r="G224" s="12"/>
+    </row>
+    <row r="225" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B225" s="12"/>
+      <c r="C225" s="12"/>
+      <c r="D225" s="12"/>
+      <c r="E225" s="12"/>
+      <c r="F225" s="12"/>
+      <c r="G225" s="12"/>
+    </row>
+    <row r="226" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B226" s="12"/>
+      <c r="C226" s="12"/>
+      <c r="D226" s="12"/>
+      <c r="E226" s="12"/>
+      <c r="F226" s="12"/>
+      <c r="G226" s="12"/>
+    </row>
+    <row r="227" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B227" s="12"/>
+      <c r="C227" s="12"/>
+      <c r="D227" s="12"/>
+      <c r="E227" s="12"/>
+      <c r="F227" s="12"/>
+      <c r="G227" s="12"/>
+    </row>
+    <row r="228" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B228" s="12"/>
+      <c r="C228" s="12"/>
+      <c r="D228" s="12"/>
+      <c r="E228" s="12"/>
+      <c r="F228" s="12"/>
+      <c r="G228" s="12"/>
+    </row>
+    <row r="229" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B229" s="12"/>
+      <c r="C229" s="12"/>
+      <c r="D229" s="12"/>
+      <c r="E229" s="12"/>
+      <c r="F229" s="12"/>
+      <c r="G229" s="12"/>
+    </row>
+    <row r="230" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B230" s="12"/>
+      <c r="C230" s="12"/>
+      <c r="D230" s="12"/>
+      <c r="E230" s="12"/>
+      <c r="F230" s="12"/>
+      <c r="G230" s="12"/>
+    </row>
+    <row r="231" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B231" s="12"/>
+      <c r="C231" s="12"/>
+      <c r="D231" s="12"/>
+      <c r="E231" s="12"/>
+      <c r="F231" s="12"/>
+      <c r="G231" s="12"/>
+    </row>
+    <row r="232" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B232" s="12"/>
+      <c r="C232" s="12"/>
+      <c r="D232" s="12"/>
+      <c r="E232" s="12"/>
+      <c r="F232" s="12"/>
+      <c r="G232" s="12"/>
+    </row>
+    <row r="233" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B233" s="12"/>
+      <c r="C233" s="12"/>
+      <c r="D233" s="12"/>
+      <c r="E233" s="12"/>
+      <c r="F233" s="12"/>
+      <c r="G233" s="12"/>
+    </row>
+    <row r="234" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B234" s="12"/>
+      <c r="C234" s="12"/>
+      <c r="D234" s="12"/>
+      <c r="E234" s="12"/>
+      <c r="F234" s="12"/>
+      <c r="G234" s="12"/>
+    </row>
+    <row r="235" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B235" s="12"/>
+      <c r="C235" s="12"/>
+      <c r="D235" s="12"/>
+      <c r="E235" s="12"/>
+      <c r="F235" s="12"/>
+      <c r="G235" s="12"/>
+    </row>
+    <row r="236" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B236" s="12"/>
+      <c r="C236" s="12"/>
+      <c r="D236" s="12"/>
+      <c r="E236" s="12"/>
+      <c r="F236" s="12"/>
+      <c r="G236" s="12"/>
+    </row>
+    <row r="237" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B237" s="12"/>
+      <c r="C237" s="12"/>
+      <c r="D237" s="12"/>
+      <c r="E237" s="12"/>
+      <c r="F237" s="12"/>
+      <c r="G237" s="12"/>
+    </row>
+    <row r="238" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B238" s="12"/>
+      <c r="C238" s="12"/>
+      <c r="D238" s="12"/>
+      <c r="E238" s="12"/>
+      <c r="F238" s="12"/>
+      <c r="G238" s="12"/>
+    </row>
+    <row r="239" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B239" s="12"/>
+      <c r="C239" s="12"/>
+      <c r="D239" s="12"/>
+      <c r="E239" s="12"/>
+      <c r="F239" s="12"/>
+      <c r="G239" s="12"/>
+    </row>
+    <row r="240" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B240" s="12"/>
+      <c r="C240" s="12"/>
+      <c r="D240" s="12"/>
+      <c r="E240" s="12"/>
+      <c r="F240" s="12"/>
+      <c r="G240" s="12"/>
+    </row>
+    <row r="241" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B241" s="12"/>
+      <c r="C241" s="12"/>
+      <c r="D241" s="12"/>
+      <c r="E241" s="12"/>
+      <c r="F241" s="12"/>
+      <c r="G241" s="12"/>
+    </row>
+    <row r="242" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B242" s="12"/>
+      <c r="C242" s="12"/>
+      <c r="D242" s="12"/>
+      <c r="E242" s="12"/>
+      <c r="F242" s="12"/>
+      <c r="G242" s="12"/>
+    </row>
+    <row r="243" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B243" s="12"/>
+      <c r="C243" s="12"/>
+      <c r="D243" s="12"/>
+      <c r="E243" s="12"/>
+      <c r="F243" s="12"/>
+      <c r="G243" s="12"/>
+    </row>
+    <row r="244" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B244" s="12"/>
+      <c r="C244" s="12"/>
+      <c r="D244" s="12"/>
+      <c r="E244" s="12"/>
+      <c r="F244" s="12"/>
+      <c r="G244" s="12"/>
+    </row>
+    <row r="245" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B245" s="12"/>
+      <c r="C245" s="12"/>
+      <c r="D245" s="12"/>
+      <c r="E245" s="12"/>
+      <c r="F245" s="12"/>
+      <c r="G245" s="12"/>
+    </row>
+    <row r="246" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B246" s="12"/>
+      <c r="C246" s="12"/>
+      <c r="D246" s="12"/>
+      <c r="E246" s="12"/>
+      <c r="F246" s="12"/>
+      <c r="G246" s="12"/>
+    </row>
+    <row r="247" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B247" s="12"/>
+      <c r="C247" s="12"/>
+      <c r="D247" s="12"/>
+      <c r="E247" s="12"/>
+      <c r="F247" s="12"/>
+      <c r="G247" s="12"/>
+    </row>
+    <row r="248" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B248" s="12"/>
+      <c r="C248" s="12"/>
+      <c r="D248" s="12"/>
+      <c r="E248" s="12"/>
+      <c r="F248" s="12"/>
+      <c r="G248" s="12"/>
+    </row>
+    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B249" s="12"/>
+      <c r="C249" s="12"/>
+      <c r="D249" s="12"/>
+      <c r="E249" s="12"/>
+      <c r="F249" s="12"/>
+      <c r="G249" s="12"/>
+    </row>
+    <row r="250" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B250" s="12"/>
+      <c r="C250" s="12"/>
+      <c r="D250" s="12"/>
+      <c r="E250" s="12"/>
+      <c r="F250" s="12"/>
+      <c r="G250" s="12"/>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B322" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>